<commit_message>
javascript hoverover, input text
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yspos\IdeaProjects\SeleniumAutomationWithJAMAL\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F839150E-2380-4882-86DE-465D39C737B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BCDA74-B2CF-4C50-8E4B-528B7852D3F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AF4E519-A2B7-45F2-9C88-52DF6CD80443}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>driver423</t>
   </si>
 </sst>
 </file>
@@ -78,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -394,13 +404,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7C5BF2-7DDC-4628-B4CD-A83E242B842B}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -416,6 +429,22 @@
       </c>
       <c r="B2">
         <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4565678899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>